<commit_message>
Atualização de artefatos da dissertação.
</commit_message>
<xml_diff>
--- a/ArtigoFormatoIEEE/EvoluçãoDVCS.xlsx
+++ b/ArtigoFormatoIEEE/EvoluçãoDVCS.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24270" windowHeight="13320"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24270" windowHeight="13320" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="Plan2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Tool</t>
   </si>
@@ -32,6 +33,18 @@
   </si>
   <si>
     <t>Mercurial</t>
+  </si>
+  <si>
+    <t>Usage per Country</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Brazil (%)</t>
   </si>
 </sst>
 </file>
@@ -78,9 +91,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,11 +547,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="229551536"/>
-        <c:axId val="229551928"/>
+        <c:axId val="231066136"/>
+        <c:axId val="231066528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="229551536"/>
+        <c:axId val="231066136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -580,7 +594,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="229551928"/>
+        <c:crossAx val="231066528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -588,7 +602,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="229551928"/>
+        <c:axId val="231066528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -639,7 +653,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="229551536"/>
+        <c:crossAx val="231066136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -720,7 +734,365 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR"/>
+              <a:t>Git</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" baseline="0"/>
+              <a:t> usage per country - Brazil's contribution</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR"/>
+              <a:t> (%)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plan2!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Brazil (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Plan2!$B$1:$E$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2012</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Plan2!$B$4:$E$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.4990953734815198E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.1488351051798235E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1218366814505609E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.8008142812402129E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="231073192"/>
+        <c:axId val="231070448"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="231073192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="231070448"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="231070448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="231073192"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1276,6 +1648,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1290,6 +2178,41 @@
       <xdr:colOff>485774</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1600,7 +2523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" activeCellId="1" sqref="E2 E5"/>
     </sheetView>
   </sheetViews>
@@ -1708,4 +2631,95 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCellId="1" sqref="A4:E4 A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1">
+        <v>2009</v>
+      </c>
+      <c r="C1">
+        <v>2010</v>
+      </c>
+      <c r="D1">
+        <v>2011</v>
+      </c>
+      <c r="E1">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>58</v>
+      </c>
+      <c r="C2">
+        <v>190</v>
+      </c>
+      <c r="D2">
+        <v>129</v>
+      </c>
+      <c r="E2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>3869</v>
+      </c>
+      <c r="C3">
+        <v>8842</v>
+      </c>
+      <c r="D3">
+        <v>11499</v>
+      </c>
+      <c r="E3">
+        <v>6386</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2">
+        <f>B2/B3</f>
+        <v>1.4990953734815198E-2</v>
+      </c>
+      <c r="C4" s="2">
+        <f t="shared" ref="C4:E4" si="0">C2/C3</f>
+        <v>2.1488351051798235E-2</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1218366814505609E-2</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" si="0"/>
+        <v>1.8008142812402129E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Atualização do Artigo no formato IEEE
</commit_message>
<xml_diff>
--- a/ArtigoFormatoIEEE/EvoluçãoDVCS.xlsx
+++ b/ArtigoFormatoIEEE/EvoluçãoDVCS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24270" windowHeight="13320" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24270" windowHeight="13320"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Tool</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Brazil (%)</t>
+  </si>
+  <si>
+    <t>fonte: https://git.wiki.kernel.org/index.php/GitSurvey2011</t>
   </si>
 </sst>
 </file>
@@ -547,11 +550,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="231066136"/>
-        <c:axId val="231066528"/>
+        <c:axId val="248830920"/>
+        <c:axId val="248832880"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="231066136"/>
+        <c:axId val="248830920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -594,7 +597,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="231066528"/>
+        <c:crossAx val="248832880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -602,7 +605,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="231066528"/>
+        <c:axId val="248832880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -653,7 +656,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="231066136"/>
+        <c:crossAx val="248830920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -897,11 +900,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="231073192"/>
-        <c:axId val="231070448"/>
+        <c:axId val="248831312"/>
+        <c:axId val="248833272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="231073192"/>
+        <c:axId val="248831312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -944,7 +947,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="231070448"/>
+        <c:crossAx val="248833272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -952,7 +955,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="231070448"/>
+        <c:axId val="248833272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1003,7 +1006,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="231073192"/>
+        <c:crossAx val="248831312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2523,7 +2526,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E5" activeCellId="1" sqref="E2 E5"/>
     </sheetView>
   </sheetViews>
@@ -2635,10 +2638,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCellId="1" sqref="A4:E4 A1:E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2718,6 +2721,11 @@
         <v>1.8008142812402129E-2</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
v1 da apresentação em português
</commit_message>
<xml_diff>
--- a/ArtigoFormatoIEEE/EvoluçãoDVCS.xlsx
+++ b/ArtigoFormatoIEEE/EvoluçãoDVCS.xlsx
@@ -94,10 +94,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -137,12 +138,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -151,13 +149,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pt-BR"/>
-              <a:t>Version Control</a:t>
+              <a:t>Version Control Usage</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="pt-BR" baseline="0"/>
-              <a:t> Usage</a:t>
-            </a:r>
-            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -175,12 +168,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -225,10 +215,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Plan1!$B$1:$E$1</c:f>
+              <c:f>Plan1!$B$1:$F$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>2010</c:v>
                 </c:pt>
@@ -240,16 +230,19 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2014</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Plan1!$B$2:$E$2</c:f>
+              <c:f>Plan1!$B$2:$F$2</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.58299999999999996</c:v>
                 </c:pt>
@@ -261,6 +254,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.378</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00%">
+                  <c:v>0.307</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -295,10 +291,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Plan1!$B$1:$E$1</c:f>
+              <c:f>Plan1!$B$1:$F$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>2010</c:v>
                 </c:pt>
@@ -310,16 +306,19 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2014</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Plan1!$B$3:$E$3</c:f>
+              <c:f>Plan1!$B$3:$F$3</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>6.8000000000000005E-2</c:v>
                 </c:pt>
@@ -331,6 +330,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.30299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.33299999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -365,10 +367,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Plan1!$B$1:$E$1</c:f>
+              <c:f>Plan1!$B$1:$F$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>2010</c:v>
                 </c:pt>
@@ -380,21 +382,27 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2014</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Plan1!$B$4:$E$4</c:f>
+              <c:f>Plan1!$B$4:$F$4</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="2">
                   <c:v>4.3999999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00%">
+                  <c:v>9.6000000000000002E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -429,10 +437,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Plan1!$B$1:$E$1</c:f>
+              <c:f>Plan1!$B$1:$F$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>2010</c:v>
                 </c:pt>
@@ -444,16 +452,19 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2014</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Plan1!$B$5:$E$5</c:f>
+              <c:f>Plan1!$B$5:$F$5</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.126</c:v>
                 </c:pt>
@@ -465,6 +476,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>4.4999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.7000000000000005E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -499,10 +513,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Plan1!$B$1:$E$1</c:f>
+              <c:f>Plan1!$B$1:$F$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>2010</c:v>
                 </c:pt>
@@ -514,16 +528,19 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2014</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Plan1!$B$6:$E$6</c:f>
+              <c:f>Plan1!$B$6:$F$6</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.03</c:v>
                 </c:pt>
@@ -535,6 +552,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>4.4999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.1000000000000001E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -550,11 +570,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="248830920"/>
-        <c:axId val="248832880"/>
+        <c:axId val="213395840"/>
+        <c:axId val="213397800"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="248830920"/>
+        <c:axId val="213395840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -582,12 +602,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -597,7 +614,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="248832880"/>
+        <c:crossAx val="213397800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -605,7 +622,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="248832880"/>
+        <c:axId val="213397800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -641,12 +658,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -656,7 +670,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="248830920"/>
+        <c:crossAx val="213395840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -684,12 +698,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -724,7 +735,11 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr b="1">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="pt-BR"/>
     </a:p>
@@ -785,7 +800,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -900,11 +914,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="248831312"/>
-        <c:axId val="248833272"/>
+        <c:axId val="213395056"/>
+        <c:axId val="284576704"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="248831312"/>
+        <c:axId val="213395056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -947,7 +961,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="248833272"/>
+        <c:crossAx val="284576704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -955,7 +969,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="248833272"/>
+        <c:axId val="284576704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1006,7 +1020,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="248831312"/>
+        <c:crossAx val="213395056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2524,15 +2538,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" activeCellId="1" sqref="E2 E5"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2548,8 +2562,11 @@
       <c r="E1">
         <v>2013</v>
       </c>
+      <c r="F1">
+        <v>2014</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2565,8 +2582,11 @@
       <c r="E2" s="1">
         <v>0.378</v>
       </c>
+      <c r="F2" s="3">
+        <v>0.307</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2582,8 +2602,11 @@
       <c r="E3" s="1">
         <v>0.30299999999999999</v>
       </c>
+      <c r="F3" s="1">
+        <v>0.33299999999999996</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2595,8 +2618,11 @@
       <c r="E4" s="1">
         <v>0.06</v>
       </c>
+      <c r="F4" s="3">
+        <v>9.6000000000000002E-2</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2612,8 +2638,11 @@
       <c r="E5" s="1">
         <v>4.4999999999999998E-2</v>
       </c>
+      <c r="F5" s="1">
+        <v>3.7000000000000005E-2</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2628,6 +2657,9 @@
       </c>
       <c r="E6" s="1">
         <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2.1000000000000001E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>